<commit_message>
For consistency, read.xlsx also returns character columns only
</commit_message>
<xml_diff>
--- a/tests/testthat/test_input.xlsx
+++ b/tests/testthat/test_input.xlsx
@@ -9,14 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16440" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16440" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="8" r:id="rId1"/>
-    <sheet name="historic data" sheetId="11" r:id="rId2"/>
-    <sheet name="entities" sheetId="6" r:id="rId3"/>
-    <sheet name="measurement model" sheetId="3" r:id="rId4"/>
-    <sheet name="config" sheetId="2" r:id="rId5"/>
+    <sheet name="entities" sheetId="6" r:id="rId2"/>
+    <sheet name="measurement model" sheetId="3" r:id="rId3"/>
+    <sheet name="config" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="124">
   <si>
     <t>Latent</t>
   </si>
@@ -400,12 +399,6 @@
   </si>
   <si>
     <t>Test 36</t>
-  </si>
-  <si>
-    <t>test_raw.xlsx</t>
-  </si>
-  <si>
-    <t>Link</t>
   </si>
 </sst>
 </file>
@@ -842,10 +835,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -858,40 +851,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>80</v>
       </c>
@@ -912,17 +880,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -933,7 +901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>71</v>
       </c>
@@ -942,7 +910,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -953,7 +921,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -964,7 +932,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -975,7 +943,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -986,7 +954,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -997,7 +965,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1008,7 +976,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1019,7 +987,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1030,7 +998,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1041,7 +1009,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1052,7 +1020,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -1063,7 +1031,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1074,7 +1042,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
@@ -1085,7 +1053,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -1096,7 +1064,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -1107,7 +1075,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
@@ -1118,7 +1086,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -1129,7 +1097,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
@@ -1140,7 +1108,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -1151,7 +1119,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1162,7 +1130,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
@@ -1173,7 +1141,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
@@ -1184,7 +1152,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
@@ -1195,7 +1163,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>20</v>
       </c>
@@ -1206,7 +1174,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
@@ -1217,7 +1185,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
@@ -1228,7 +1196,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>20</v>
       </c>
@@ -1239,7 +1207,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>35</v>
       </c>
@@ -1250,7 +1218,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
@@ -1261,7 +1229,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>35</v>
       </c>
@@ -1272,7 +1240,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>35</v>
       </c>
@@ -1283,7 +1251,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>35</v>
       </c>
@@ -1294,7 +1262,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>41</v>
       </c>
@@ -1305,7 +1273,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>41</v>
       </c>
@@ -1316,7 +1284,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>41</v>
       </c>
@@ -1327,7 +1295,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>4</v>
       </c>
@@ -1349,17 +1317,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -1370,7 +1338,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1381,7 +1349,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -1392,7 +1360,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1403,7 +1371,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -1414,7 +1382,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1425,7 +1393,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -1436,7 +1404,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -1447,7 +1415,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>49</v>
       </c>
@@ -1458,7 +1426,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>49</v>
       </c>
@@ -1469,7 +1437,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -1480,7 +1448,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -1491,7 +1459,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -1502,7 +1470,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -1513,7 +1481,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -1524,7 +1492,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -1535,7 +1503,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -1546,7 +1514,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -1557,7 +1525,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>69</v>
       </c>

</xml_diff>